<commit_message>
update dev version of userguide
</commit_message>
<xml_diff>
--- a/CSVs/myXL.xlsx
+++ b/CSVs/myXL.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adrian\Documents\GitHub\DLMtool_UserGuide\CSVs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23370" windowHeight="10470" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23370" windowHeight="10470" tabRatio="830" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Example1Stock" sheetId="1" r:id="rId1"/>
     <sheet name="Example1Fleet" sheetId="2" r:id="rId2"/>
     <sheet name="Example1Obs" sheetId="3" r:id="rId3"/>
-    <sheet name="Example2Stock" sheetId="4" r:id="rId4"/>
-    <sheet name="Example2Fleet" sheetId="5" r:id="rId5"/>
-    <sheet name="Example2Obs" sheetId="6" r:id="rId6"/>
+    <sheet name="Example1Imp" sheetId="7" r:id="rId4"/>
+    <sheet name="Example2Stock" sheetId="4" r:id="rId5"/>
+    <sheet name="Example2Fleet" sheetId="5" r:id="rId6"/>
+    <sheet name="Example2Obs" sheetId="6" r:id="rId7"/>
+    <sheet name="Example2Imp" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -24,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -249,13 +256,37 @@
   </si>
   <si>
     <t>Esd</t>
+  </si>
+  <si>
+    <t>TACSD</t>
+  </si>
+  <si>
+    <t>TACFrac</t>
+  </si>
+  <si>
+    <t>ESD</t>
+  </si>
+  <si>
+    <t>EFrac</t>
+  </si>
+  <si>
+    <t>SizeLimSD</t>
+  </si>
+  <si>
+    <t>SizeLimFrac</t>
+  </si>
+  <si>
+    <t>DLMtool generated</t>
+  </si>
+  <si>
+    <t>Perfect_Imp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,13 +294,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -284,9 +327,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1385,6 +1431,106 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="39" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1671,11 +1817,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1830,7 +1976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
@@ -2165,4 +2311,105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="A1:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>